<commit_message>
Update version to 0.1.0 Remove some cards from the excel sheet
</commit_message>
<xml_diff>
--- a/Winterhold-cards.xlsx
+++ b/Winterhold-cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/StS-Winterhold/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA5F5B0-1AF1-364E-9241-BFF6ACBF9E73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E577D0A-4C70-5F48-8E9C-EB147076EA29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15960" yWindow="-21140" windowWidth="34720" windowHeight="21140" xr2:uid="{23C39FC3-D53D-7C45-B446-56A09C7C2148}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
   <si>
     <t>Energy</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Deal 1 Frost damage 4(6) times.</t>
   </si>
   <si>
-    <t>Ground</t>
-  </si>
-  <si>
     <t>Elemental Flow</t>
   </si>
   <si>
@@ -171,27 +168,9 @@
     <t>Sparks</t>
   </si>
   <si>
-    <t>Deal 8(11) Shock damage to a random enemy.</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
-    <t>HoseDown</t>
-  </si>
-  <si>
-    <t>OilUp</t>
-  </si>
-  <si>
-    <t>Apply 2(3) Resistance to Shock and 2(3) Vulnerable to Frost.</t>
-  </si>
-  <si>
-    <t>Apply 2(3) Resistance to Frost and 2(3) Vulnerable to Fire.</t>
-  </si>
-  <si>
-    <t>Apply 2(3) Resistance to Fire and 2(3) Vulnerable to Shock.</t>
-  </si>
-  <si>
     <t>Simon Says</t>
   </si>
   <si>
@@ -244,6 +223,9 @@
   </si>
   <si>
     <t>Frost Rune</t>
+  </si>
+  <si>
+    <t>Deal 8 Shock damage to ALL enemies.</t>
   </si>
 </sst>
 </file>
@@ -961,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FEE2E7-935E-3C44-BB4E-9F2FEF1FFA75}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -990,10 +972,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
@@ -1054,7 +1036,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>12</v>
@@ -1092,7 +1074,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>13</v>
@@ -1109,7 +1091,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1">
         <f>COUNTIF(E2:E90, "Uncommon")</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O4" s="1"/>
     </row>
@@ -1130,7 +1112,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>14</v>
@@ -1168,7 +1150,7 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>15</v>
@@ -1188,7 +1170,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1">
         <f>SUBTOTAL(109,Table24[Destruction])</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="O6" s="1"/>
     </row>
@@ -1209,7 +1191,7 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -1220,7 +1202,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1229,7 +1211,7 @@
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>19</v>
@@ -1255,19 +1237,22 @@
     </row>
     <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>20</v>
@@ -1290,13 +1275,13 @@
     </row>
     <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1305,7 +1290,7 @@
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>21</v>
@@ -1322,19 +1307,19 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1">
         <f>COUNTIF(B2:B90, "Skill")</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1343,7 +1328,7 @@
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>22</v>
@@ -1366,13 +1351,13 @@
     </row>
     <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1381,7 +1366,7 @@
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>15</v>
@@ -1407,13 +1392,13 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1424,13 +1409,13 @@
     </row>
     <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1462,13 +1447,13 @@
     </row>
     <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1497,13 +1482,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1532,13 +1517,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1547,7 +1532,7 @@
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
@@ -1564,7 +1549,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1">
         <f>COUNTIF(D2:D90,"=1")</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O17" s="1"/>
     </row>
@@ -1629,6 +1614,21 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
       <c r="I21" s="1" t="s">
         <v>15</v>
       </c>
@@ -1647,111 +1647,40 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1">
         <f>SUM(Table2[Destruction])</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="O21" s="1"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I24" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J24" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="I25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
         <v>51</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" t="s">
-        <v>46</v>
-      </c>
-      <c r="I25" t="s">
-        <v>55</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="J26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" t="s">
-        <v>46</v>
-      </c>
-      <c r="I26" t="s">
-        <v>58</v>
-      </c>
-      <c r="J26" t="s">
-        <v>64</v>
-      </c>
-    </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" t="s">
-        <v>46</v>
-      </c>
       <c r="I27" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" t="s">
         <v>53</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Balance: buff fireball Ignore xlsx open-file
</commit_message>
<xml_diff>
--- a/Winterhold-cards.xlsx
+++ b/Winterhold-cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/StS-Winterhold/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E577D0A-4C70-5F48-8E9C-EB147076EA29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130A45BB-457B-194E-91CA-18A20E0DE467}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15960" yWindow="-21140" windowWidth="34720" windowHeight="21140" xr2:uid="{23C39FC3-D53D-7C45-B446-56A09C7C2148}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
   <si>
     <t>Energy</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Chain Lightning</t>
   </si>
   <si>
-    <t>Deal 6(7) Fire damage to yourself. Deal 36(42) Fire damage.</t>
-  </si>
-  <si>
     <t>Apply 1(2) Jumpy Lightning.</t>
   </si>
   <si>
@@ -225,7 +222,10 @@
     <t>Frost Rune</t>
   </si>
   <si>
-    <t>Deal 8 Shock damage to ALL enemies.</t>
+    <t>Deal 8(11) Shock damage to ALL enemies.</t>
+  </si>
+  <si>
+    <t>Deal 6 Fire damage to yourself. Deal 36(42) Fire damage.</t>
   </si>
 </sst>
 </file>
@@ -946,7 +946,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,10 +972,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
         <v>59</v>
-      </c>
-      <c r="G1" t="s">
-        <v>60</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
@@ -1036,7 +1036,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>12</v>
@@ -1074,7 +1074,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>13</v>
@@ -1112,7 +1112,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>14</v>
@@ -1150,7 +1150,7 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>15</v>
@@ -1191,7 +1191,7 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -1202,16 +1202,16 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>19</v>
@@ -1243,7 +1243,7 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1252,7 +1252,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>20</v>
@@ -1290,7 +1290,7 @@
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>21</v>
@@ -1313,13 +1313,13 @@
     </row>
     <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1328,7 +1328,7 @@
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>22</v>
@@ -1357,7 +1357,7 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1366,7 +1366,7 @@
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>15</v>
@@ -1398,7 +1398,7 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1406,16 +1406,19 @@
       <c r="E13" t="s">
         <v>12</v>
       </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1447,13 +1450,13 @@
     </row>
     <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1482,13 +1485,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1517,13 +1520,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1532,7 +1535,7 @@
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
@@ -1569,7 +1572,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1">
         <f>COUNTIF(D2:D90,"=2")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O18" s="1"/>
     </row>
@@ -1589,7 +1592,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1">
         <f>COUNTIF(D2:D90,"=3")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O19" s="1"/>
     </row>
@@ -1615,13 +1618,13 @@
     </row>
     <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1653,34 +1656,34 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I27" t="s">
+        <v>51</v>
+      </c>
+      <c r="J27" t="s">
         <v>52</v>
-      </c>
-      <c r="J27" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more card ideas
</commit_message>
<xml_diff>
--- a/Winterhold-cards.xlsx
+++ b/Winterhold-cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/StS-Winterhold/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130A45BB-457B-194E-91CA-18A20E0DE467}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533BBDAC-5045-1C49-800B-09478BF1B6A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15960" yWindow="-21140" windowWidth="34720" windowHeight="21140" xr2:uid="{23C39FC3-D53D-7C45-B446-56A09C7C2148}"/>
+    <workbookView xWindow="520" yWindow="860" windowWidth="34720" windowHeight="21140" xr2:uid="{23C39FC3-D53D-7C45-B446-56A09C7C2148}"/>
   </bookViews>
   <sheets>
     <sheet name="Destruction" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
   <si>
     <t>Energy</t>
   </si>
@@ -111,12 +111,6 @@
     <t>Deal 6(9) Fire damage.</t>
   </si>
   <si>
-    <t>Deal 5 Frost damage. Apply 1(2) Weak.</t>
-  </si>
-  <si>
-    <t>Deal 3 Shock damage. Apply 2(3) Vulnerable.</t>
-  </si>
-  <si>
     <t>Gain 5 Block.</t>
   </si>
   <si>
@@ -226,6 +220,27 @@
   </si>
   <si>
     <t>Deal 6 Fire damage to yourself. Deal 36(42) Fire damage.</t>
+  </si>
+  <si>
+    <t>Gain 4(7) Block. The next time you're attacked, deal 4(7) Fire damage back.</t>
+  </si>
+  <si>
+    <t>Deal 5 Shock damage. Apply 1(2) Vulnerable.</t>
+  </si>
+  <si>
+    <t>Deal 5(7) Frost damage. Gain 5(7) Block.</t>
+  </si>
+  <si>
+    <t>Cold Burn</t>
+  </si>
+  <si>
+    <t>Deal 5(7) Frost damage. Deal 5(7) Fire damage.</t>
+  </si>
+  <si>
+    <t>Hypothermia</t>
+  </si>
+  <si>
+    <t>Gain 10 Block. Shuffle a Void into your draw pile.</t>
   </si>
 </sst>
 </file>
@@ -946,7 +961,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,10 +987,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
@@ -1021,7 +1036,7 @@
     </row>
     <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -1036,7 +1051,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>12</v>
@@ -1053,7 +1068,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1">
         <f>COUNTIF(E2:E90, "Common")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O3" s="1"/>
     </row>
@@ -1065,7 +1080,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1074,7 +1089,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>13</v>
@@ -1091,19 +1106,19 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1">
         <f>COUNTIF(E2:E90, "Uncommon")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1112,7 +1127,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>14</v>
@@ -1141,7 +1156,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1150,7 +1165,7 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>15</v>
@@ -1170,19 +1185,19 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1">
         <f>SUBTOTAL(109,Table24[Destruction])</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1191,18 +1206,18 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1211,7 +1226,7 @@
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>19</v>
@@ -1237,13 +1252,13 @@
     </row>
     <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1252,7 +1267,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>20</v>
@@ -1269,19 +1284,19 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1">
         <f>COUNTIF(B2:B90, "Attack")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1290,7 +1305,7 @@
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>21</v>
@@ -1307,19 +1322,19 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1">
         <f>COUNTIF(B2:B90, "Skill")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1328,7 +1343,7 @@
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>22</v>
@@ -1351,13 +1366,13 @@
     </row>
     <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1366,7 +1381,7 @@
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>15</v>
@@ -1392,13 +1407,13 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1407,18 +1422,18 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1427,7 +1442,7 @@
         <v>12</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>9</v>
@@ -1450,13 +1465,13 @@
     </row>
     <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1464,8 +1479,11 @@
       <c r="E15" t="s">
         <v>12</v>
       </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
       <c r="I15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J15" s="1">
         <v>3</v>
@@ -1485,13 +1503,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1514,19 +1532,19 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1">
         <f>COUNTIF(D2:D90,"=0")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1535,7 +1553,7 @@
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
@@ -1552,11 +1570,29 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1">
         <f>COUNTIF(D2:D90,"=1")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
       <c r="I18" s="1">
         <v>2</v>
       </c>
@@ -1577,6 +1613,24 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
       <c r="I19" s="1">
         <v>3</v>
       </c>
@@ -1597,8 +1651,23 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
       <c r="I20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J20" s="1">
         <v>1</v>
@@ -1617,21 +1686,6 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
       <c r="I21" s="1" t="s">
         <v>15</v>
       </c>
@@ -1650,40 +1704,40 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1">
         <f>SUM(Table2[Destruction])</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="O21" s="1"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" t="s">
         <v>46</v>
-      </c>
-      <c r="J24" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I25" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" t="s">
         <v>47</v>
-      </c>
-      <c r="J25" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add temporary backgrounds for all cards Card system overhaul
</commit_message>
<xml_diff>
--- a/Winterhold-cards.xlsx
+++ b/Winterhold-cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/StS-Winterhold/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8DCAD3-BF86-DA4D-A132-B0622D19F4F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2425BE5-734C-7340-BD08-63F7C1DC309B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="460" windowWidth="34720" windowHeight="21940" xr2:uid="{23C39FC3-D53D-7C45-B446-56A09C7C2148}"/>
   </bookViews>
@@ -873,9 +873,6 @@
     <t>Enemy Summon 2: Kill this to receive 20 gold.</t>
   </si>
   <si>
-    <t>Remove 5 Block. Deal 5 damage.</t>
-  </si>
-  <si>
     <t>Conjure Ice Knife</t>
   </si>
   <si>
@@ -892,6 +889,9 @@
   </si>
   <si>
     <t>Choose a card from your hand to Capture. Summon 2: Play a copy of that card.</t>
+  </si>
+  <si>
+    <t>Remove 5 Block from the enemy. Deal 5 damage.</t>
   </si>
 </sst>
 </file>
@@ -1576,8 +1576,8 @@
   <dimension ref="A1:P212"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3064,7 +3064,7 @@
         <v>19</v>
       </c>
       <c r="C49" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3269,13 +3269,13 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B80" t="s">
         <v>20</v>
       </c>
       <c r="C80" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -3286,13 +3286,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B81" t="s">
         <v>20</v>
       </c>
       <c r="C81" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -3727,13 +3727,13 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B152" t="s">
         <v>19</v>
       </c>
       <c r="C152" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D152">
         <v>2</v>

</xml_diff>